<commit_message>
Da thay doi test/DuLieuDoThi_Euler_Book.xlsx ( 1 thanh o & o thanh 1)
</commit_message>
<xml_diff>
--- a/DuLieuDoThi_Euler_Book.xlsx
+++ b/DuLieuDoThi_Euler_Book.xlsx
@@ -25960,7 +25960,7 @@
   <dimension ref="A2:X29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -26080,32 +26080,32 @@
         <v>0</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
-        <v>0</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0</v>
-      </c>
       <c r="K5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="14">
         <f>COUNTIF(E5:M5,"&lt;&gt;0")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="29"/>
       <c r="S5" s="27"/>
@@ -26453,35 +26453,35 @@
       </c>
       <c r="F15" s="14">
         <f t="shared" ref="F15:M15" si="1">COUNTIF(F5:F13,"&lt;&gt;0")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G15" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H15" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J15" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K15" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L15" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M15" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="29"/>
       <c r="S15" s="27"/>
@@ -28269,12 +28269,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="L1:L3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="K1:K3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:B3"/>
@@ -28291,6 +28285,12 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="K1:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>